<commit_message>
Count Dooku und die Mediclorianer
</commit_message>
<xml_diff>
--- a/Dokumentation/Plan/Projektplan.xlsx
+++ b/Dokumentation/Plan/Projektplan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Projektplan Homepage</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Legende:</t>
   </si>
   <si>
-    <t>Kai</t>
-  </si>
-  <si>
-    <t>Oliver</t>
-  </si>
-  <si>
     <t>Beide</t>
   </si>
   <si>
@@ -84,14 +78,38 @@
     <t>Scribble</t>
   </si>
   <si>
-    <t>Feinkonzept</t>
+    <t>Designentwurf</t>
+  </si>
+  <si>
+    <t>Farbkonzept</t>
+  </si>
+  <si>
+    <t>Design Photoshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSS </t>
+  </si>
+  <si>
+    <t>Inhaltsfindung</t>
+  </si>
+  <si>
+    <t>Hauptsächlich Kai</t>
+  </si>
+  <si>
+    <t>Hauptsächlich Oliver</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Inhalt ins XML</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +137,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -183,12 +208,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -204,7 +230,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -278,7 +304,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -313,7 +338,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -489,179 +513,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="37" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="3.42578125" customWidth="1"/>
-    <col min="42" max="42" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.77734375" customWidth="1"/>
+    <col min="4" max="37" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="3.44140625" customWidth="1"/>
+    <col min="42" max="42" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:42" ht="25.8">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:42">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>40759</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>40760</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="9">
         <v>40761</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="9">
         <v>40762</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="9">
         <v>40763</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="9">
         <v>40764</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="9">
         <v>40765</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="9">
         <v>40766</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="9">
         <v>40767</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="9">
         <v>40768</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="9">
         <v>40769</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="9">
         <v>40770</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="9">
         <v>40771</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="9">
         <v>40772</v>
       </c>
-      <c r="R2" s="8">
+      <c r="R2" s="9">
         <v>40773</v>
       </c>
-      <c r="S2" s="8">
+      <c r="S2" s="9">
         <v>40774</v>
       </c>
-      <c r="T2" s="8">
+      <c r="T2" s="9">
         <v>40775</v>
       </c>
-      <c r="U2" s="8">
+      <c r="U2" s="9">
         <v>40776</v>
       </c>
-      <c r="V2" s="8">
+      <c r="V2" s="9">
         <v>40777</v>
       </c>
-      <c r="W2" s="8">
+      <c r="W2" s="9">
         <v>40778</v>
       </c>
-      <c r="X2" s="8">
+      <c r="X2" s="9">
         <v>40779</v>
       </c>
-      <c r="Y2" s="8">
+      <c r="Y2" s="9">
         <v>40780</v>
       </c>
-      <c r="Z2" s="8">
+      <c r="Z2" s="9">
         <v>40781</v>
       </c>
-      <c r="AA2" s="8">
+      <c r="AA2" s="9">
         <v>40782</v>
       </c>
-      <c r="AB2" s="8">
+      <c r="AB2" s="9">
         <v>40783</v>
       </c>
-      <c r="AC2" s="8">
+      <c r="AC2" s="9">
         <v>40784</v>
       </c>
-      <c r="AD2" s="8">
+      <c r="AD2" s="9">
         <v>40785</v>
       </c>
-      <c r="AE2" s="8">
+      <c r="AE2" s="9">
         <v>40786</v>
       </c>
-      <c r="AF2" s="8">
+      <c r="AF2" s="9">
         <v>40787</v>
       </c>
-      <c r="AG2" s="8">
+      <c r="AG2" s="9">
         <v>40788</v>
       </c>
-      <c r="AH2" s="8">
+      <c r="AH2" s="9">
         <v>40789</v>
       </c>
-      <c r="AI2" s="8">
+      <c r="AI2" s="9">
         <v>40790</v>
       </c>
-      <c r="AJ2" s="8">
+      <c r="AJ2" s="9">
         <v>40791</v>
       </c>
-      <c r="AK2" s="8">
+      <c r="AK2" s="9">
         <v>40792</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" ht="49.5" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="8"/>
-      <c r="AK3" s="8"/>
-    </row>
-    <row r="4" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
+    </row>
+    <row r="4" spans="1:42" ht="18">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -671,55 +695,61 @@
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="8"/>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+    </row>
+    <row r="5" spans="1:42">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="5"/>
@@ -727,96 +757,275 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3"/>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="5"/>
       <c r="AO7" s="2"/>
       <c r="AP7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="AK8" s="5"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42">
       <c r="AO8" s="4"/>
       <c r="AP8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="AO9" s="3"/>
       <c r="AP9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="N10" s="5"/>
-      <c r="AO10" s="5"/>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="5"/>
+      <c r="AO10" t="s">
+        <v>11</v>
+      </c>
       <c r="AP10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
       <c r="N11" s="5"/>
-      <c r="AO11" s="1"/>
+      <c r="AO11" s="5"/>
       <c r="AP11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="M12" s="10"/>
       <c r="N12" s="5"/>
-      <c r="AO12" t="s">
-        <v>11</v>
-      </c>
+      <c r="AO12" s="1"/>
       <c r="AP12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="5"/>
+      <c r="AO13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:42">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="N13" s="5"/>
-      <c r="AO13" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:42">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+    </row>
+    <row r="17" spans="1:37">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="5"/>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="4"/>
+      <c r="AE18" s="4"/>
+    </row>
+    <row r="19" spans="1:37">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="W19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="5"/>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="AP13" t="s">
-        <v>14</v>
-      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="AK2:AK4"/>
+    <mergeCell ref="AE2:AE4"/>
+    <mergeCell ref="AF2:AF4"/>
+    <mergeCell ref="AG2:AG4"/>
+    <mergeCell ref="AH2:AH4"/>
+    <mergeCell ref="AI2:AI4"/>
+    <mergeCell ref="AJ2:AJ4"/>
+    <mergeCell ref="AD2:AD4"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="T2:T4"/>
+    <mergeCell ref="U2:U4"/>
+    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="AB2:AB4"/>
+    <mergeCell ref="AC2:AC4"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
@@ -833,25 +1042,6 @@
     <mergeCell ref="O2:O4"/>
     <mergeCell ref="P2:P4"/>
     <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="AD2:AD4"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="T2:T4"/>
-    <mergeCell ref="U2:U4"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="AB2:AB4"/>
-    <mergeCell ref="AC2:AC4"/>
-    <mergeCell ref="AK2:AK4"/>
-    <mergeCell ref="AE2:AE4"/>
-    <mergeCell ref="AF2:AF4"/>
-    <mergeCell ref="AG2:AG4"/>
-    <mergeCell ref="AH2:AH4"/>
-    <mergeCell ref="AI2:AI4"/>
-    <mergeCell ref="AJ2:AJ4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -859,24 +1049,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>